<commit_message>
first part sprint 4
</commit_message>
<xml_diff>
--- a/Calibration.xlsx
+++ b/Calibration.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanKennedy/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanKennedy/Documents/GitHub/KNW-Robot-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>